<commit_message>
Panty: Targeted lines for Tomoko, Megumin, and Nami
**Total Linecount: ** 1269 -> 1310 (+41)
**Generic Linecount: ** 579 -> 581 (+2)
**Special-Conditions Linecount: ** 64 -> 82 (+18)
**Targeted Linecount: ** 516 -> 553 (+37)
**Referenced Poses: ** 157 -> 158 (+1)
**Total Targeted Characters: ** 61 -> 63 (+2)

Targeting Updates:
    - `jessie`: 46 -> 49 (+3)
    - `meia`: 2 -> 3 (+1)
    - `human`: 37 -> 39 (+2)
    - `nami`: 2 -> 10 (+8)
    - `megumin`: 28 -> 34 (+6)
    - `maki`: 0 -> 2 (+2)
    - `tomoko`: 0 -> 16 (+16)

Command executed by: Arndress#7172
</commit_message>
<xml_diff>
--- a/opponents/panty/Panty Model Rework.xlsx
+++ b/opponents/panty/Panty Model Rework.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shani\Documents\GitHub\spnati\opponents\panty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy Wikie\Downloads\SPnati\spnati\opponents\panty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4C10F6-AEEB-4A9F-8F6A-6351345180AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52C277B-29FE-4FE3-8D4E-437C903F6AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9990" yWindow="1560" windowWidth="17685" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>